<commit_message>
Modificações de atributos nome e descrição em produto + documentação do projeto
</commit_message>
<xml_diff>
--- a/Dicionário de Dados.xlsx
+++ b/Dicionário de Dados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Documents\Faculdade\Tópicos Integradores II\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Documents\Faculdade\Tópicos Integradores II\T-picos-Integradores-II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6435C3A-40F3-4A0E-B317-B5D9F0B71A7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABB5FA6-35A5-4677-BBF8-B8AE3B07560E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A9DA61B-806C-4F21-B725-0CD8BBE438DD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="128">
   <si>
     <t>Tabela</t>
   </si>
@@ -63,9 +63,6 @@
     <t>integer</t>
   </si>
   <si>
-    <t>not null; auto_increent; primary key; unique</t>
-  </si>
-  <si>
     <t>nome_cliente</t>
   </si>
   <si>
@@ -406,6 +403,18 @@
   </si>
   <si>
     <t>not null; &gt; 0</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>varchar(300)</t>
+  </si>
+  <si>
+    <t>nome do produto</t>
+  </si>
+  <si>
+    <t>descrição do produto</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7827AC62-75DF-4F7B-9C13-4E58649687DC}">
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90:D95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,178 +842,178 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1016,10 +1026,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1030,7 +1040,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>7</v>
@@ -1038,16 +1048,16 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1058,10 +1068,10 @@
         <v>9</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1074,10 +1084,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1088,7 +1098,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>7</v>
@@ -1096,114 +1106,114 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C34" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C37" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,10 +1226,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>7</v>
@@ -1238,30 +1248,30 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1274,10 +1284,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,7 +1298,7 @@
         <v>5</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>7</v>
@@ -1296,170 +1306,170 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C53" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="C54" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C56" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C58" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C59" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C61" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1472,10 +1482,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,7 +1496,7 @@
         <v>5</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>7</v>
@@ -1494,30 +1504,30 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1530,10 +1540,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1544,7 +1554,7 @@
         <v>5</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>7</v>
@@ -1552,230 +1562,258 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D74" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>9</v>
+      <c r="B75" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>104</v>
+      <c r="A76" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B78" s="2" t="s">
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="C87" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D83" s="1" t="s">
+      <c r="C92" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>13</v>
+      <c r="C96" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unificacao do campo cpf e cnpj
</commit_message>
<xml_diff>
--- a/Dicionário de Dados.xlsx
+++ b/Dicionário de Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Documents\Faculdade\Tópicos Integradores II\T-picos-Integradores-II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABB5FA6-35A5-4677-BBF8-B8AE3B07560E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FA5530-2653-4279-949A-CC1E1DED854A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A9DA61B-806C-4F21-B725-0CD8BBE438DD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="128">
   <si>
     <t>Tabela</t>
   </si>
@@ -123,12 +123,6 @@
     <t>char(7)</t>
   </si>
   <si>
-    <t>cnpj</t>
-  </si>
-  <si>
-    <t>char(14)</t>
-  </si>
-  <si>
     <t>tipo_cliente</t>
   </si>
   <si>
@@ -243,9 +237,6 @@
     <t>Sigla do estado onde o cliente reside</t>
   </si>
   <si>
-    <t>Cpf do cliente</t>
-  </si>
-  <si>
     <t>Rg do cliente caso seja pessoa física</t>
   </si>
   <si>
@@ -255,9 +246,6 @@
     <t>Número do telefone do cliente</t>
   </si>
   <si>
-    <t>Cnpj do cliente caso seja pessoa jurídica</t>
-  </si>
-  <si>
     <t>Identificador do cliente</t>
   </si>
   <si>
@@ -415,6 +403,18 @@
   </si>
   <si>
     <t>descrição do produto</t>
+  </si>
+  <si>
+    <t>cpf_cnpj</t>
+  </si>
+  <si>
+    <t>vatchar(14)</t>
+  </si>
+  <si>
+    <t>Cpf ou cnpj do cliente</t>
+  </si>
+  <si>
+    <t>unique</t>
   </si>
 </sst>
 </file>
@@ -790,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7827AC62-75DF-4F7B-9C13-4E58649687DC}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,10 +842,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -856,7 +856,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -870,7 +870,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
@@ -884,7 +884,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -898,7 +898,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -912,7 +912,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -926,7 +926,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -940,7 +940,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -954,7 +954,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -962,13 +962,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>15</v>
@@ -982,10 +982,10 @@
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -993,115 +993,115 @@
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>7</v>
+      <c r="C22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="2" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1109,24 +1109,24 @@
         <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>12</v>
@@ -1134,13 +1134,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>12</v>
@@ -1148,13 +1148,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>12</v>
@@ -1162,13 +1162,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>12</v>
@@ -1176,13 +1176,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>12</v>
@@ -1190,157 +1190,157 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="2" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>7</v>
+      <c r="C42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="2" t="s">
+      <c r="B46" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>7</v>
+      <c r="C49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>15</v>
@@ -1348,13 +1348,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>15</v>
@@ -1362,27 +1362,27 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>12</v>
@@ -1390,13 +1390,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>12</v>
@@ -1404,13 +1404,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>12</v>
@@ -1418,13 +1418,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>12</v>
@@ -1432,13 +1432,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>12</v>
@@ -1446,373 +1446,359 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>12</v>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="A63" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B66" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C67" s="2" t="s">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B68" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>7</v>
+      <c r="C73" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>9</v>
+      <c r="A74" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>46</v>
+        <v>120</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>125</v>
+      <c r="A76" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B80" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D80" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>7</v>
+      <c r="D85" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B87" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>7</v>
+      <c r="C92" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C94" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D97" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Alteracao no atributo de Fornecedor + atributos do diagrama de classes
</commit_message>
<xml_diff>
--- a/Dicionário de Dados.xlsx
+++ b/Dicionário de Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Documents\Faculdade\Tópicos Integradores II\T-picos-Integradores-II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FA5530-2653-4279-949A-CC1E1DED854A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8A39ED-970A-40B3-A230-ED7B528E170C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A9DA61B-806C-4F21-B725-0CD8BBE438DD}"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="20265" windowHeight="10755" xr2:uid="{9A9DA61B-806C-4F21-B725-0CD8BBE438DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="129">
   <si>
     <t>Tabela</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t>unique</t>
+  </si>
+  <si>
+    <t>Email do fornecedor</t>
   </si>
 </sst>
 </file>
@@ -790,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7827AC62-75DF-4F7B-9C13-4E58649687DC}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,27 +1123,27 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>12</v>
@@ -1148,13 +1151,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>12</v>
@@ -1162,13 +1165,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>12</v>
@@ -1176,13 +1179,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>12</v>
@@ -1190,157 +1193,157 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="D37" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>15</v>
@@ -1348,13 +1351,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>15</v>
@@ -1362,27 +1365,27 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>12</v>
@@ -1390,13 +1393,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>12</v>
@@ -1404,13 +1407,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>12</v>
@@ -1418,13 +1421,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>12</v>
@@ -1432,13 +1435,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>12</v>
@@ -1446,359 +1449,373 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="D61" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="D76" s="2" t="s">
-        <v>103</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C86" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Relatórios pedido por George
</commit_message>
<xml_diff>
--- a/Dicionário de Dados.xlsx
+++ b/Dicionário de Dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Documents\Faculdade\Tópicos Integradores II\T-picos-Integradores-II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8A39ED-970A-40B3-A230-ED7B528E170C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A4A169-7E2B-4999-817B-A01882B24275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="165" windowWidth="20265" windowHeight="10755" xr2:uid="{9A9DA61B-806C-4F21-B725-0CD8BBE438DD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="130">
   <si>
     <t>Tabela</t>
   </si>
@@ -417,7 +417,10 @@
     <t>unique</t>
   </si>
   <si>
-    <t>Email do fornecedor</t>
+    <t>data_pedido</t>
+  </si>
+  <si>
+    <t>Data de realização do pedido</t>
   </si>
 </sst>
 </file>
@@ -793,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7827AC62-75DF-4F7B-9C13-4E58649687DC}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1132,7 @@
         <v>14</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>128</v>
+        <v>73</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>15</v>
@@ -1719,103 +1722,117 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>